<commit_message>
Importaciones de Procesadores - Memorias
</commit_message>
<xml_diff>
--- a/public/importar/processors.xlsx
+++ b/public/importar/processors.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">usersabs</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">Usuario</t>
   </si>
   <si>
     <t xml:space="preserve">Service Tag</t>
@@ -43,10 +43,16 @@
     <t xml:space="preserve">ddclass</t>
   </si>
   <si>
+    <t xml:space="preserve">usuario1@tmp.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRJYJ01</t>
   </si>
   <si>
     <t xml:space="preserve">00:00:00:00:00:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usuario2@tmp.com</t>
   </si>
   <si>
     <t xml:space="preserve">KCR3MGX</t>
@@ -104,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -129,14 +135,21 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -182,11 +195,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +213,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -325,178 +346,190 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>16757551</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>66677276</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>66863664</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>66863664</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>66863664</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>66863664</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>66863664</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>66863664</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>66996031</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="usuario1@tmp.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="usuario2@tmp.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="usuario1@tmp.com"/>
+    <hyperlink ref="A5" r:id="rId4" display="usuario2@tmp.com"/>
+    <hyperlink ref="A6" r:id="rId5" display="usuario1@tmp.com"/>
+    <hyperlink ref="A7" r:id="rId6" display="usuario2@tmp.com"/>
+    <hyperlink ref="A8" r:id="rId7" display="usuario1@tmp.com"/>
+    <hyperlink ref="A9" r:id="rId8" display="usuario2@tmp.com"/>
+    <hyperlink ref="A10" r:id="rId9" display="usuario2@tmp.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
CRUD Procesadores - Selects dependientes
</commit_message>
<xml_diff>
--- a/public/importar/processors.xlsx
+++ b/public/importar/processors.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">memories_add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity_addmem</t>
+    <t xml:space="preserve">memories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
   </si>
   <si>
     <t xml:space="preserve">prototype_reference</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">00:00:00:00:00:01</t>
   </si>
   <si>
-    <t xml:space="preserve">nanya_pc2-4200U-444-12-A1</t>
+    <t xml:space="preserve">SN001</t>
   </si>
   <si>
     <t xml:space="preserve">Referencia-01</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">00:00:00:00:00:02</t>
   </si>
   <si>
-    <t xml:space="preserve">kingston_pc2-4200U-444-12-B1</t>
+    <t xml:space="preserve">SN002</t>
   </si>
   <si>
     <t xml:space="preserve">Referencia-02</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">00:00:00:00:00:04</t>
   </si>
   <si>
-    <t xml:space="preserve">nanya_pc2-4200U-444-12-A1,mct_pc2-3200U-333-10-A1</t>
+    <t xml:space="preserve">SN004,SN005</t>
   </si>
   <si>
     <t xml:space="preserve">Referencia-04</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">00:00:00:00:00:06</t>
   </si>
   <si>
-    <t xml:space="preserve">mac_pc3-10600U-09-10-B0,kingston_pc2-4200U-444-12-B1</t>
+    <t xml:space="preserve">SN005,SN006</t>
   </si>
   <si>
     <t xml:space="preserve">Referencia-06</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">00:00:00:00:00:10</t>
   </si>
   <si>
-    <t xml:space="preserve">Fjeoeoe-eoeoeoeo</t>
+    <t xml:space="preserve">SN003</t>
   </si>
   <si>
     <t xml:space="preserve">Referencia-10</t>
@@ -161,7 +161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -202,6 +202,11 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -246,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -271,11 +276,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,7 +418,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,7 +428,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -456,17 +465,17 @@
         <v>9</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -477,13 +486,13 @@
         <v>14</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -498,13 +507,13 @@
         <v>18</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="6" t="s">
+      <c r="E4" s="0"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -515,13 +524,13 @@
         <v>21</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="7" t="n">
         <v>3.1</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -537,12 +546,12 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -553,13 +562,13 @@
         <v>28</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="7" t="n">
         <v>5.2</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -575,8 +584,8 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="6" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -592,8 +601,8 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -609,8 +618,8 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -624,14 +633,14 @@
       <c r="C11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>